<commit_message>
Modification de la gestion des quantité de repas offert pour les artistes et les benevoles
</commit_message>
<xml_diff>
--- a/assets/tickets_repas_MS09.xlsx
+++ b/assets/tickets_repas_MS09.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projets\Programmation\Morphoz_SnackApp\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{936A0394-7D76-431F-9576-88E7C81EC5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1D4F9C-B8B5-4189-B2DE-EC530C614618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3BB1B9DD-3069-430A-BC8B-4311BE1E654B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3BB1B9DD-3069-430A-BC8B-4311BE1E654B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
   <si>
     <t>Adélie POITIERS</t>
   </si>
@@ -134,10 +134,10 @@
     <t>Catégorie</t>
   </si>
   <si>
-    <t>20/06/2025</t>
-  </si>
-  <si>
-    <t>21/06/2025</t>
+    <t>Nathan ISON</t>
+  </si>
+  <si>
+    <t>Quantité</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0&quot; h&quot;"/>
+    <numFmt numFmtId="164" formatCode="0&quot; h&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -182,32 +182,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -216,6 +204,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -231,17 +222,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EE89698-7EB3-44F4-AF1D-2C3227728025}" name="Tableau1" displayName="Tableau1" ref="A1:D29" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:D29" xr:uid="{0EE89698-7EB3-44F4-AF1D-2C3227728025}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
-    <sortCondition ref="B2:B29"/>
-    <sortCondition ref="A2:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0EE89698-7EB3-44F4-AF1D-2C3227728025}" name="Tableau1" displayName="Tableau1" ref="A1:C30" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="A1:C30" xr:uid="{0EE89698-7EB3-44F4-AF1D-2C3227728025}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C30">
+    <sortCondition ref="B2:B30"/>
+    <sortCondition ref="A2:A30"/>
   </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{36BE445F-755C-4249-9D03-177D23356A66}" name="Nom" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{9F6773AE-EB7D-4497-8934-8B7A5BFD8924}" name="Catégorie" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{86DC95CF-B2B3-45FB-B759-DCF581971385}" name="20/06/2025" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6727C3CA-0AF9-4680-96F8-75415AF645DA}" name="21/06/2025" dataDxfId="1"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{36BE445F-755C-4249-9D03-177D23356A66}" name="Nom" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{9F6773AE-EB7D-4497-8934-8B7A5BFD8924}" name="Catégorie" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3D46917D-10F8-4CCB-848C-D5346E92FD4C}" name="Quantité" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -544,86 +534,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5207C94-F20A-451B-A7B2-0718B8E4C51E}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="4" customWidth="1"/>
-    <col min="3" max="4" width="12.85546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="51" customWidth="1"/>
+    <col min="1" max="1" width="27.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="51" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -632,22 +614,20 @@
       <c r="C6" s="1">
         <v>1</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -656,293 +636,204 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="1">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="1">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
-      </c>
-      <c r="D27" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
-      </c>
-      <c r="D28" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>1</v>
-      </c>
+      <c r="B30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>